<commit_message>
Made some more tweaks after testing with data on BeastOfRennaLab.  Deleted unneeded template workbooks now that everything is auto generating!
</commit_message>
<xml_diff>
--- a/Excel_Macros/Cell_Units_Template.xlsx
+++ b/Excel_Macros/Cell_Units_Template.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook1" defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dan_Programming\Programs\MEA-Cruncher\Old_Scripts\Excel_Macros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dan_Programming\Programs\WaveAnalysisScripts\Excel_Macros\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OFS_Entry" sheetId="8" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>Noise Cutoff:</t>
   </si>
   <si>
-    <t>Use the Noise Cutoff cell on the next sheet to quickly identify potential noise units based on their number of spikes</t>
-  </si>
-  <si>
     <t>PotentialNoise</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Noise?</t>
+  </si>
+  <si>
+    <t>You can use the Noise Cutoff cell on the next sheet to quickly identify potential noise units based on their number of spikes</t>
   </si>
 </sst>
 </file>
@@ -363,8 +363,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="OFSTbl" displayName="OFSTbl" ref="A10:J11" insertRow="1" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A10:J11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="OFSTbl" displayName="OFSTbl" ref="A9:J10" insertRow="1" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A9:J10"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Channel" dataDxfId="19"/>
     <tableColumn id="2" name="Waveforms" dataDxfId="18"/>
@@ -671,10 +671,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,55 +716,52 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A7" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
+      <c r="J9" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -775,9 +773,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H484"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -823,10 +822,10 @@
         <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>0</v>
@@ -12141,7 +12140,7 @@
         <v>56</v>
       </c>
       <c r="B457" s="14">
-        <f t="shared" ref="B457:B488" si="17">MOD(ROW(A457)-5,MaxUnits)</f>
+        <f t="shared" ref="B457:B484" si="17">MOD(ROW(A457)-5,MaxUnits)</f>
         <v>4</v>
       </c>
       <c r="C457" s="14" t="str">

</xml_diff>

<commit_message>
Add some tiny columns to make pasting OFS data into the Cell_Units_Template easier.  Added gitignore lines for workbooks generated from the templates
</commit_message>
<xml_diff>
--- a/Excel_Macros/Cell_Units_Template.xlsx
+++ b/Excel_Macros/Cell_Units_Template.xlsx
@@ -287,15 +287,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -365,6 +356,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -392,45 +392,45 @@
   <tableColumns count="13">
     <tableColumn id="1" name="Name" dataDxfId="23"/>
     <tableColumn id="2" name="Samples" dataDxfId="22"/>
-    <tableColumn id="13" name="Waveforms" dataDxfId="0"/>
-    <tableColumn id="12" name="Blank" dataDxfId="1"/>
-    <tableColumn id="11" name="Unsorted" dataDxfId="2"/>
-    <tableColumn id="3" name="a" dataDxfId="21"/>
-    <tableColumn id="4" name="b" dataDxfId="20"/>
-    <tableColumn id="5" name="c" dataDxfId="19"/>
-    <tableColumn id="6" name="d" dataDxfId="18"/>
-    <tableColumn id="7" name="e" dataDxfId="17"/>
-    <tableColumn id="8" name="f" dataDxfId="16"/>
-    <tableColumn id="9" name="g" dataDxfId="15"/>
-    <tableColumn id="10" name="h" dataDxfId="14"/>
+    <tableColumn id="13" name="Waveforms" dataDxfId="21"/>
+    <tableColumn id="12" name="Blank" dataDxfId="20"/>
+    <tableColumn id="11" name="Unsorted" dataDxfId="19"/>
+    <tableColumn id="3" name="a" dataDxfId="18"/>
+    <tableColumn id="4" name="b" dataDxfId="17"/>
+    <tableColumn id="5" name="c" dataDxfId="16"/>
+    <tableColumn id="6" name="d" dataDxfId="15"/>
+    <tableColumn id="7" name="e" dataDxfId="14"/>
+    <tableColumn id="8" name="f" dataDxfId="13"/>
+    <tableColumn id="9" name="g" dataDxfId="12"/>
+    <tableColumn id="10" name="h" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ValidationTbl" displayName="ValidationTbl" ref="A4:I484" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ValidationTbl" displayName="ValidationTbl" ref="A4:I484" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A4:I484"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="RowOffset" dataDxfId="11">
+    <tableColumn id="1" name="RowOffset" dataDxfId="8">
       <calculatedColumnFormula>_xlfn.FLOOR.MATH((ROW(A5)-5)/MaxUnits)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="ColOffset" dataDxfId="10">
+    <tableColumn id="2" name="ColOffset" dataDxfId="7">
       <calculatedColumnFormula>MOD(ROW(A5)-5,MaxUnits)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="UnitName" dataDxfId="9">
+    <tableColumn id="3" name="UnitName" dataDxfId="6">
       <calculatedColumnFormula>OFFSET(OFSTbl[Name],ValidationTbl[[#This Row],[RowOffset]],0,1,1)&amp;OFFSET(OFSTbl[[#Headers],[a]],0,ValidationTbl[[#This Row],[ColOffset]],1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="NumSpikes" dataDxfId="8">
+    <tableColumn id="4" name="NumSpikes" dataDxfId="5">
       <calculatedColumnFormula>OFFSET(OFSTbl[a],ValidationTbl[[#This Row],[RowOffset]],ValidationTbl[[#This Row],[ColOffset]],1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="PotentialNoise" dataDxfId="7">
+    <tableColumn id="5" name="PotentialNoise" dataDxfId="4">
       <calculatedColumnFormula>IF(ValidationTbl[[#This Row],[NumSpikes]]&lt;NoiseCutoff,"x","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Bad?" dataDxfId="6"/>
-    <tableColumn id="6" name="ipRGC?" dataDxfId="5"/>
-    <tableColumn id="7" name="Same?" dataDxfId="4"/>
-    <tableColumn id="9" name="KickOut?" dataDxfId="3"/>
+    <tableColumn id="8" name="Bad?" dataDxfId="3"/>
+    <tableColumn id="6" name="ipRGC?" dataDxfId="2"/>
+    <tableColumn id="7" name="Same?" dataDxfId="1"/>
+    <tableColumn id="9" name="KickOut?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -702,14 +702,16 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="0.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="0.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="5" style="1" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Fixed tissue ID lookups for property values/STTCs
</commit_message>
<xml_diff>
--- a/Excel_Macros/Cell_Units_Template.xlsx
+++ b/Excel_Macros/Cell_Units_Template.xlsx
@@ -16,8 +16,8 @@
     <sheet name="Validation" sheetId="9" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="MaxUnits">Validation!$B$1</definedName>
-    <definedName name="NoiseCutoff">Validation!$B$2</definedName>
+    <definedName name="MaxUnits">Validation!$D$1</definedName>
+    <definedName name="NoiseCutoff">Validation!$D$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -287,54 +287,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -373,6 +325,54 @@
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -387,50 +387,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="OFSTbl" displayName="OFSTbl" ref="A9:M10" insertRow="1" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="OFSTbl" displayName="OFSTbl" ref="A9:M10" insertRow="1" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A9:M10"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Name" dataDxfId="23"/>
-    <tableColumn id="2" name="Samples" dataDxfId="22"/>
-    <tableColumn id="13" name="Waveforms" dataDxfId="21"/>
-    <tableColumn id="12" name="Blank" dataDxfId="20"/>
-    <tableColumn id="11" name="Unsorted" dataDxfId="19"/>
-    <tableColumn id="3" name="a" dataDxfId="18"/>
-    <tableColumn id="4" name="b" dataDxfId="17"/>
-    <tableColumn id="5" name="c" dataDxfId="16"/>
-    <tableColumn id="6" name="d" dataDxfId="15"/>
-    <tableColumn id="7" name="e" dataDxfId="14"/>
-    <tableColumn id="8" name="f" dataDxfId="13"/>
-    <tableColumn id="9" name="g" dataDxfId="12"/>
-    <tableColumn id="10" name="h" dataDxfId="11"/>
+    <tableColumn id="1" name="Name" dataDxfId="12"/>
+    <tableColumn id="2" name="Samples" dataDxfId="11"/>
+    <tableColumn id="13" name="Waveforms" dataDxfId="10"/>
+    <tableColumn id="12" name="Blank" dataDxfId="9"/>
+    <tableColumn id="11" name="Unsorted" dataDxfId="8"/>
+    <tableColumn id="3" name="a" dataDxfId="7"/>
+    <tableColumn id="4" name="b" dataDxfId="6"/>
+    <tableColumn id="5" name="c" dataDxfId="5"/>
+    <tableColumn id="6" name="d" dataDxfId="4"/>
+    <tableColumn id="7" name="e" dataDxfId="3"/>
+    <tableColumn id="8" name="f" dataDxfId="2"/>
+    <tableColumn id="9" name="g" dataDxfId="1"/>
+    <tableColumn id="10" name="h" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ValidationTbl" displayName="ValidationTbl" ref="A4:I484" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ValidationTbl" displayName="ValidationTbl" ref="A4:I484" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A4:I484"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="RowOffset" dataDxfId="8">
+    <tableColumn id="1" name="RowOffset" dataDxfId="23">
       <calculatedColumnFormula>_xlfn.FLOOR.MATH((ROW(A5)-5)/MaxUnits)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="ColOffset" dataDxfId="7">
+    <tableColumn id="2" name="ColOffset" dataDxfId="22">
       <calculatedColumnFormula>MOD(ROW(A5)-5,MaxUnits)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="UnitName" dataDxfId="6">
+    <tableColumn id="3" name="UnitName" dataDxfId="21">
       <calculatedColumnFormula>OFFSET(OFSTbl[Name],ValidationTbl[[#This Row],[RowOffset]],0,1,1)&amp;OFFSET(OFSTbl[[#Headers],[a]],0,ValidationTbl[[#This Row],[ColOffset]],1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="NumSpikes" dataDxfId="5">
+    <tableColumn id="4" name="NumSpikes" dataDxfId="20">
       <calculatedColumnFormula>OFFSET(OFSTbl[a],ValidationTbl[[#This Row],[RowOffset]],ValidationTbl[[#This Row],[ColOffset]],1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="PotentialNoise" dataDxfId="4">
+    <tableColumn id="5" name="PotentialNoise" dataDxfId="19">
       <calculatedColumnFormula>IF(ValidationTbl[[#This Row],[NumSpikes]]&lt;NoiseCutoff,"x","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Bad?" dataDxfId="3"/>
-    <tableColumn id="6" name="ipRGC?" dataDxfId="2"/>
-    <tableColumn id="7" name="Same?" dataDxfId="1"/>
-    <tableColumn id="9" name="KickOut?" dataDxfId="0"/>
+    <tableColumn id="8" name="Bad?" dataDxfId="18"/>
+    <tableColumn id="6" name="ipRGC?" dataDxfId="17"/>
+    <tableColumn id="7" name="Same?" dataDxfId="16"/>
+    <tableColumn id="9" name="KickOut?" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -703,7 +703,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,12 +820,14 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I484"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="5" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="5" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
@@ -837,18 +839,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="13">
+      <c r="D1" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="10">
+      <c r="D2" s="10">
         <v>400</v>
       </c>
     </row>

</xml_diff>